<commit_message>
Batter vs team done
</commit_message>
<xml_diff>
--- a/archive/bowler_team_data(2022).xlsx
+++ b/archive/bowler_team_data(2022).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kannan-PC\Desktop\MS\Projects\fantasyer\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C229A6-E19C-44C3-8AD6-B0D776B16E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DBEEF3-B80D-4E11-A4BB-6C56C8D33607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{ACEDE91F-F8B9-4C81-ACE2-B4190679E489}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="122">
   <si>
     <t>TS Mills</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>R Parag</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Bowlers</t>
   </si>
 </sst>
 </file>
@@ -764,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DEC483-4918-4B5A-B7DE-667893B3658E}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,10 +785,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +804,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -806,7 +812,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -830,7 +836,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +844,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -846,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,15 +860,15 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -870,7 +876,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -878,7 +884,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -886,7 +892,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,7 +900,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +908,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -910,7 +916,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -918,7 +924,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -926,7 +932,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -934,7 +940,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -942,7 +948,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -950,15 +956,15 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -966,7 +972,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,7 +980,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -982,7 +988,7 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +996,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -998,7 +1004,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,7 +1012,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1014,7 +1020,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1028,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1030,7 +1036,7 @@
         <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1038,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1046,7 +1052,7 @@
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1060,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,7 +1068,7 @@
         <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1070,15 +1076,15 @@
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1086,7 +1092,7 @@
         <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,7 +1100,7 @@
         <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1102,7 +1108,7 @@
         <v>57</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1110,7 +1116,7 @@
         <v>57</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1118,7 +1124,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1126,7 +1132,7 @@
         <v>57</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1134,7 +1140,7 @@
         <v>57</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1142,7 +1148,7 @@
         <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1150,7 +1156,7 @@
         <v>57</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,15 +1164,15 @@
         <v>57</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1180,7 @@
         <v>82</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1182,7 +1188,7 @@
         <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1190,7 +1196,7 @@
         <v>82</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1204,7 @@
         <v>82</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,7 +1212,7 @@
         <v>82</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1214,7 +1220,7 @@
         <v>82</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,7 +1228,7 @@
         <v>82</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1230,7 +1236,7 @@
         <v>82</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1238,7 +1244,7 @@
         <v>82</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1246,15 +1252,15 @@
         <v>82</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,7 +1268,7 @@
         <v>25</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1270,7 +1276,7 @@
         <v>25</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1278,7 +1284,7 @@
         <v>25</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1286,7 +1292,7 @@
         <v>25</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1294,7 +1300,7 @@
         <v>25</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1302,7 +1308,7 @@
         <v>25</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1310,7 +1316,7 @@
         <v>25</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1318,7 +1324,7 @@
         <v>25</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1326,7 +1332,7 @@
         <v>25</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1334,7 +1340,7 @@
         <v>25</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1342,7 +1348,7 @@
         <v>25</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1350,7 +1356,7 @@
         <v>25</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1358,7 +1364,7 @@
         <v>25</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1366,15 +1372,15 @@
         <v>25</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1382,7 +1388,7 @@
         <v>58</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1390,7 +1396,7 @@
         <v>58</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1398,7 +1404,7 @@
         <v>58</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,7 +1412,7 @@
         <v>58</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1414,7 +1420,7 @@
         <v>58</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1422,7 +1428,7 @@
         <v>58</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,7 +1436,7 @@
         <v>58</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1438,15 +1444,15 @@
         <v>58</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1454,7 +1460,7 @@
         <v>59</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1462,7 +1468,7 @@
         <v>59</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1470,7 +1476,7 @@
         <v>59</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1484,7 @@
         <v>59</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1486,7 +1492,7 @@
         <v>59</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1494,7 +1500,7 @@
         <v>59</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1502,7 +1508,7 @@
         <v>59</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1510,7 +1516,7 @@
         <v>59</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1518,15 +1524,15 @@
         <v>59</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1534,7 +1540,7 @@
         <v>60</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1542,7 +1548,7 @@
         <v>60</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1550,7 +1556,7 @@
         <v>60</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1558,7 +1564,7 @@
         <v>60</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>110</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1566,7 +1572,7 @@
         <v>60</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1574,7 +1580,7 @@
         <v>60</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1582,7 +1588,7 @@
         <v>60</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1590,15 +1596,15 @@
         <v>60</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1606,7 +1612,7 @@
         <v>61</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1614,7 +1620,7 @@
         <v>61</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1622,7 +1628,7 @@
         <v>61</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -1630,7 +1636,7 @@
         <v>61</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1638,7 +1644,7 @@
         <v>61</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1652,7 @@
         <v>61</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -1654,6 +1660,14 @@
         <v>61</v>
       </c>
       <c r="B110" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added batter vs team and bowler vs team
</commit_message>
<xml_diff>
--- a/archive/bowler_team_data(2022).xlsx
+++ b/archive/bowler_team_data(2022).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kannan-PC\Desktop\MS\Projects\fantasyer\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DBEEF3-B80D-4E11-A4BB-6C56C8D33607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20A9E1E-5DF0-43B1-AB07-0A7C383D6FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{ACEDE91F-F8B9-4C81-ACE2-B4190679E489}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="137">
   <si>
     <t>TS Mills</t>
   </si>
@@ -401,23 +401,61 @@
   </si>
   <si>
     <t>Bowlers</t>
+  </si>
+  <si>
+    <t>DJ Mitchell</t>
+  </si>
+  <si>
+    <t>Navdeep Saini</t>
+  </si>
+  <si>
+    <t>YBK Jaiswal</t>
+  </si>
+  <si>
+    <t>NM Coulter-Nile</t>
+  </si>
+  <si>
+    <t>M Pathirana</t>
+  </si>
+  <si>
+    <t>PH Solanki</t>
+  </si>
+  <si>
+    <t>TU Deshpande</t>
+  </si>
+  <si>
+    <t>S Dube</t>
+  </si>
+  <si>
+    <t>AF Milne</t>
+  </si>
+  <si>
+    <t>SS Iyer</t>
+  </si>
+  <si>
+    <t>Aman Hakim Khan</t>
+  </si>
+  <si>
+    <t>D Brevis</t>
+  </si>
+  <si>
+    <t>V Shankar</t>
+  </si>
+  <si>
+    <t>VG Arora</t>
+  </si>
+  <si>
+    <t>R Powell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,11 +487,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -770,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DEC483-4918-4B5A-B7DE-667893B3658E}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,882 +830,1002 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>61</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>61</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>4</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>0</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>16</v>
+      <c r="B38" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>73</v>
+        <v>15</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>75</v>
+        <v>15</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>76</v>
+        <v>15</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>77</v>
+        <v>15</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>78</v>
+        <v>57</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>81</v>
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B66" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="B78" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B79" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B69" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>101</v>
+        <v>25</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>102</v>
+        <v>25</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>103</v>
+        <v>25</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>7</v>
+        <v>25</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>104</v>
+        <v>25</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>105</v>
+        <v>58</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>106</v>
+        <v>58</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>107</v>
+        <v>58</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>108</v>
+        <v>58</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>109</v>
+        <v>58</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>110</v>
+        <v>58</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>111</v>
+        <v>58</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>112</v>
+        <v>58</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>113</v>
+        <v>59</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>114</v>
+        <v>59</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>115</v>
+        <v>59</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>116</v>
+        <v>59</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>117</v>
+        <v>59</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>118</v>
+        <v>59</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>119</v>
+        <v>59</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>